<commit_message>
Update patient example import file with new data
</commit_message>
<xml_diff>
--- a/example_import_files/patient_examples.xlsx
+++ b/example_import_files/patient_examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markj/Documents/Studium/Master Maschinenbau TH Koeln/Digitalisierung/SAPV_route_optimization/example_import_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDE667C-8A0B-054E-85FD-A1C4090C4096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9F894D-5454-564E-8F10-C9457501EDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20180" xr2:uid="{5CDA6B10-105F-5448-B8D6-FAC426D99158}"/>
   </bookViews>
@@ -343,9 +343,6 @@
     <t>Weiß</t>
   </si>
   <si>
-    <t>Tannenstraße 28</t>
-  </si>
-  <si>
     <t>Pappelstraße 25</t>
   </si>
   <si>
@@ -422,6 +419,9 @@
   </si>
   <si>
     <t>Lärchenweg 1</t>
+  </si>
+  <si>
+    <t>Lüdenscheider Straße 2</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>11</v>
@@ -1380,7 +1380,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2">
         <v>51645</v>
@@ -1433,7 +1433,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3">
         <v>51643</v>
@@ -1486,7 +1486,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4">
         <v>51645</v>
@@ -1504,31 +1504,31 @@
         <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K4" t="s">
         <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O4" t="s">
         <v>17</v>
       </c>
       <c r="P4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q4" t="s">
         <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1539,7 +1539,7 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5">
         <v>51674</v>
@@ -1577,7 +1577,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6">
         <v>51702</v>
@@ -1630,13 +1630,13 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7">
         <v>51688</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
         <v>38</v>
@@ -1648,31 +1648,31 @@
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K7" t="s">
         <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M7" t="s">
         <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O7" t="s">
         <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q7" t="s">
         <v>21</v>
       </c>
       <c r="R7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1683,7 +1683,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8">
         <v>51674</v>
@@ -1721,7 +1721,7 @@
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9">
         <v>51643</v>
@@ -1759,13 +1759,13 @@
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10">
         <v>51688</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F10" t="s">
         <v>47</v>
@@ -1812,7 +1812,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11">
         <v>51674</v>
@@ -1850,7 +1850,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12">
         <v>51643</v>
@@ -1888,7 +1888,7 @@
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13">
         <v>51643</v>
@@ -1941,7 +1941,7 @@
         <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14">
         <v>51647</v>
@@ -1982,13 +1982,13 @@
         <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15">
         <v>51688</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" t="s">
         <v>64</v>
@@ -2035,7 +2035,7 @@
         <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16">
         <v>51674</v>
@@ -2070,7 +2070,7 @@
         <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17">
         <v>51647</v>
@@ -2108,13 +2108,13 @@
         <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18">
         <v>51688</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
@@ -2129,31 +2129,31 @@
         <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" t="s">
         <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M18" t="s">
         <v>17</v>
       </c>
       <c r="N18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O18" t="s">
         <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q18" t="s">
         <v>17</v>
       </c>
       <c r="R18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19">
         <v>51674</v>
@@ -2255,13 +2255,13 @@
         <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="D21">
         <v>51688</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
         <v>83</v>
@@ -2387,7 +2387,7 @@
         <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24">
         <v>51647</v>
@@ -2440,31 +2440,31 @@
         <v>17</v>
       </c>
       <c r="J25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K25" t="s">
         <v>17</v>
       </c>
       <c r="L25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M25" t="s">
         <v>17</v>
       </c>
       <c r="N25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O25" t="s">
         <v>17</v>
       </c>
       <c r="P25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q25" t="s">
         <v>17</v>
       </c>
       <c r="R25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -2475,7 +2475,7 @@
         <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26">
         <v>51702</v>

</xml_diff>